<commit_message>
First supported opcode - 0xEA JMP r16:16 Simple utils and begin of documentation
</commit_message>
<xml_diff>
--- a/test/memory map.xlsx
+++ b/test/memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Numer bloku</t>
   </si>
@@ -25,6 +25,27 @@
   </si>
   <si>
     <t>do</t>
+  </si>
+  <si>
+    <t>0xFE000</t>
+  </si>
+  <si>
+    <t>start PC</t>
+  </si>
+  <si>
+    <t>0xFFFF0</t>
+  </si>
+  <si>
+    <t>adres w pliku BIOS</t>
+  </si>
+  <si>
+    <t>0x1FF0</t>
+  </si>
+  <si>
+    <t>przesunięcie</t>
+  </si>
+  <si>
+    <t>początek biosu w pamięci</t>
   </si>
 </sst>
 </file>
@@ -81,12 +102,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -392,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,25 +424,25 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="str">
+      <c r="B2" s="2" t="str">
         <f>DEC2HEX(A2)</f>
         <v>0</v>
       </c>
@@ -429,7 +450,7 @@
         <f>A2*64*1024</f>
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="D2" s="2" t="str">
         <f>DEC2HEX(C2)</f>
         <v>0</v>
       </c>
@@ -437,7 +458,7 @@
         <f>(A2+1)*64*1024-1</f>
         <v>65535</v>
       </c>
-      <c r="F2" s="3" t="str">
+      <c r="F2" s="2" t="str">
         <f>DEC2HEX(E2)</f>
         <v>FFFF</v>
       </c>
@@ -446,7 +467,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="str">
+      <c r="B3" s="2" t="str">
         <f t="shared" ref="B3:B17" si="0">DEC2HEX(A3)</f>
         <v>1</v>
       </c>
@@ -454,7 +475,7 @@
         <f t="shared" ref="C3:C17" si="1">A3*64*1024</f>
         <v>65536</v>
       </c>
-      <c r="D3" s="3" t="str">
+      <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D17" si="2">DEC2HEX(C3)</f>
         <v>10000</v>
       </c>
@@ -462,7 +483,7 @@
         <f t="shared" ref="E3:E17" si="3">(A3+1)*64*1024-1</f>
         <v>131071</v>
       </c>
-      <c r="F3" s="3" t="str">
+      <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F17" si="4">DEC2HEX(E3)</f>
         <v>1FFFF</v>
       </c>
@@ -471,7 +492,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="str">
+      <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -479,7 +500,7 @@
         <f t="shared" si="1"/>
         <v>131072</v>
       </c>
-      <c r="D4" s="3" t="str">
+      <c r="D4" s="2" t="str">
         <f t="shared" si="2"/>
         <v>20000</v>
       </c>
@@ -487,7 +508,7 @@
         <f t="shared" si="3"/>
         <v>196607</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="F4" s="2" t="str">
         <f t="shared" si="4"/>
         <v>2FFFF</v>
       </c>
@@ -496,7 +517,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="str">
+      <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -504,7 +525,7 @@
         <f t="shared" si="1"/>
         <v>196608</v>
       </c>
-      <c r="D5" s="3" t="str">
+      <c r="D5" s="2" t="str">
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
@@ -512,7 +533,7 @@
         <f t="shared" si="3"/>
         <v>262143</v>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="F5" s="2" t="str">
         <f t="shared" si="4"/>
         <v>3FFFF</v>
       </c>
@@ -521,7 +542,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="str">
+      <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -529,7 +550,7 @@
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-      <c r="D6" s="3" t="str">
+      <c r="D6" s="2" t="str">
         <f t="shared" si="2"/>
         <v>40000</v>
       </c>
@@ -537,7 +558,7 @@
         <f t="shared" si="3"/>
         <v>327679</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="F6" s="2" t="str">
         <f t="shared" si="4"/>
         <v>4FFFF</v>
       </c>
@@ -546,7 +567,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="str">
+      <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -554,7 +575,7 @@
         <f t="shared" si="1"/>
         <v>327680</v>
       </c>
-      <c r="D7" s="3" t="str">
+      <c r="D7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>50000</v>
       </c>
@@ -562,7 +583,7 @@
         <f t="shared" si="3"/>
         <v>393215</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="F7" s="2" t="str">
         <f t="shared" si="4"/>
         <v>5FFFF</v>
       </c>
@@ -571,7 +592,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="str">
+      <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -579,7 +600,7 @@
         <f t="shared" si="1"/>
         <v>393216</v>
       </c>
-      <c r="D8" s="3" t="str">
+      <c r="D8" s="2" t="str">
         <f t="shared" si="2"/>
         <v>60000</v>
       </c>
@@ -587,7 +608,7 @@
         <f t="shared" si="3"/>
         <v>458751</v>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="F8" s="2" t="str">
         <f t="shared" si="4"/>
         <v>6FFFF</v>
       </c>
@@ -596,7 +617,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="str">
+      <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -604,7 +625,7 @@
         <f t="shared" si="1"/>
         <v>458752</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="D9" s="2" t="str">
         <f t="shared" si="2"/>
         <v>70000</v>
       </c>
@@ -612,7 +633,7 @@
         <f t="shared" si="3"/>
         <v>524287</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="F9" s="2" t="str">
         <f t="shared" si="4"/>
         <v>7FFFF</v>
       </c>
@@ -621,7 +642,7 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="str">
+      <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -629,7 +650,7 @@
         <f t="shared" si="1"/>
         <v>524288</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D10" s="2" t="str">
         <f t="shared" si="2"/>
         <v>80000</v>
       </c>
@@ -637,7 +658,7 @@
         <f t="shared" si="3"/>
         <v>589823</v>
       </c>
-      <c r="F10" s="3" t="str">
+      <c r="F10" s="2" t="str">
         <f t="shared" si="4"/>
         <v>8FFFF</v>
       </c>
@@ -646,7 +667,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="str">
+      <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -654,7 +675,7 @@
         <f t="shared" si="1"/>
         <v>589824</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D11" s="2" t="str">
         <f t="shared" si="2"/>
         <v>90000</v>
       </c>
@@ -662,7 +683,7 @@
         <f t="shared" si="3"/>
         <v>655359</v>
       </c>
-      <c r="F11" s="3" t="str">
+      <c r="F11" s="2" t="str">
         <f t="shared" si="4"/>
         <v>9FFFF</v>
       </c>
@@ -671,7 +692,7 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="str">
+      <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
@@ -679,7 +700,7 @@
         <f t="shared" si="1"/>
         <v>655360</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>A0000</v>
       </c>
@@ -687,7 +708,7 @@
         <f t="shared" si="3"/>
         <v>720895</v>
       </c>
-      <c r="F12" s="3" t="str">
+      <c r="F12" s="2" t="str">
         <f t="shared" si="4"/>
         <v>AFFFF</v>
       </c>
@@ -696,7 +717,7 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="str">
+      <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
@@ -704,7 +725,7 @@
         <f t="shared" si="1"/>
         <v>720896</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>B0000</v>
       </c>
@@ -712,7 +733,7 @@
         <f t="shared" si="3"/>
         <v>786431</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="F13" s="2" t="str">
         <f t="shared" si="4"/>
         <v>BFFFF</v>
       </c>
@@ -721,7 +742,7 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="str">
+      <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
@@ -729,7 +750,7 @@
         <f t="shared" si="1"/>
         <v>786432</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
         <v>C0000</v>
       </c>
@@ -737,7 +758,7 @@
         <f t="shared" si="3"/>
         <v>851967</v>
       </c>
-      <c r="F14" s="3" t="str">
+      <c r="F14" s="2" t="str">
         <f t="shared" si="4"/>
         <v>CFFFF</v>
       </c>
@@ -746,7 +767,7 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="str">
+      <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
@@ -754,7 +775,7 @@
         <f t="shared" si="1"/>
         <v>851968</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
         <v>D0000</v>
       </c>
@@ -762,7 +783,7 @@
         <f t="shared" si="3"/>
         <v>917503</v>
       </c>
-      <c r="F15" s="3" t="str">
+      <c r="F15" s="2" t="str">
         <f t="shared" si="4"/>
         <v>DFFFF</v>
       </c>
@@ -771,7 +792,7 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="str">
+      <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
@@ -779,7 +800,7 @@
         <f t="shared" si="1"/>
         <v>917504</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D16" s="2" t="str">
         <f t="shared" si="2"/>
         <v>E0000</v>
       </c>
@@ -787,7 +808,7 @@
         <f t="shared" si="3"/>
         <v>983039</v>
       </c>
-      <c r="F16" s="3" t="str">
+      <c r="F16" s="2" t="str">
         <f t="shared" si="4"/>
         <v>EFFFF</v>
       </c>
@@ -796,7 +817,7 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="str">
+      <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -804,7 +825,7 @@
         <f t="shared" si="1"/>
         <v>983040</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="2" t="str">
         <f t="shared" si="2"/>
         <v>F0000</v>
       </c>
@@ -812,7 +833,7 @@
         <f t="shared" si="3"/>
         <v>1048575</v>
       </c>
-      <c r="F17" s="3" t="str">
+      <c r="F17" s="2" t="str">
         <f t="shared" si="4"/>
         <v>FFFFF</v>
       </c>
@@ -833,13 +854,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>